<commit_message>
poland, malaysia, Thailand done
</commit_message>
<xml_diff>
--- a/list of countrie.xlsx
+++ b/list of countrie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armaan/Developer/Delicious-Descoveries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vrishab Shenvi\Desktop\Web Dev\Minipro DD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F4EB40-1C41-BD4C-BFDC-EC1A17A24677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA824E5F-DEEE-403A-8E98-05BCD0A5866A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="19660" xr2:uid="{EB6D4232-37E0-D34F-B3A8-46FAD6E4D2CC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EB6D4232-37E0-D34F-B3A8-46FAD6E4D2CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="342">
   <si>
     <t>India</t>
   </si>
@@ -924,6 +924,165 @@
   </si>
   <si>
     <t>Chole Bhature</t>
+  </si>
+  <si>
+    <t>Pierogi</t>
+  </si>
+  <si>
+    <t>Bigos</t>
+  </si>
+  <si>
+    <t>Żurek</t>
+  </si>
+  <si>
+    <t>Placki Ziemniaczane</t>
+  </si>
+  <si>
+    <t>Golabki</t>
+  </si>
+  <si>
+    <t>Makowiec</t>
+  </si>
+  <si>
+    <t>Barszcz</t>
+  </si>
+  <si>
+    <t>Sernik</t>
+  </si>
+  <si>
+    <t>Kopytka</t>
+  </si>
+  <si>
+    <t>Kaczka</t>
+  </si>
+  <si>
+    <t>Sałatka Jarzynowa</t>
+  </si>
+  <si>
+    <t>Fasolka Po Bretonsku</t>
+  </si>
+  <si>
+    <t>Nalesniki</t>
+  </si>
+  <si>
+    <t>Sernik na Zimno</t>
+  </si>
+  <si>
+    <t>Zrazy</t>
+  </si>
+  <si>
+    <t>Zupa Krem z Pomidorow</t>
+  </si>
+  <si>
+    <t>Krupnik</t>
+  </si>
+  <si>
+    <t>Torty</t>
+  </si>
+  <si>
+    <t>Zurek z Biala Kielbasa</t>
+  </si>
+  <si>
+    <t>Smazony Serek</t>
+  </si>
+  <si>
+    <t>Tom Yum Goong</t>
+  </si>
+  <si>
+    <t>Green Curry</t>
+  </si>
+  <si>
+    <t>Massaman Curry</t>
+  </si>
+  <si>
+    <t>Larb</t>
+  </si>
+  <si>
+    <t>Khao Pad</t>
+  </si>
+  <si>
+    <t>Gaeng Daeng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Satay</t>
+  </si>
+  <si>
+    <t>Thai Spring Rolls</t>
+  </si>
+  <si>
+    <t>Khao Soi</t>
+  </si>
+  <si>
+    <t>Thai Iced Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moo Pad Krapow </t>
+  </si>
+  <si>
+    <t>Thai Fish Cakes</t>
+  </si>
+  <si>
+    <t>Pineapple Fried Rice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaeng Som </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jok </t>
+  </si>
+  <si>
+    <t>Sticky Rice with Mango</t>
+  </si>
+  <si>
+    <t>Roti</t>
+  </si>
+  <si>
+    <t>som tum</t>
+  </si>
+  <si>
+    <t>Panang curry</t>
+  </si>
+  <si>
+    <t>Nasi Lemak</t>
+  </si>
+  <si>
+    <t>Char Kway Teow</t>
+  </si>
+  <si>
+    <t>Beef Rendang</t>
+  </si>
+  <si>
+    <t>Chicken Satay</t>
+  </si>
+  <si>
+    <t>Roti Canai</t>
+  </si>
+  <si>
+    <t>Hainanese Chicken Rice</t>
+  </si>
+  <si>
+    <t>Mee Goreng</t>
+  </si>
+  <si>
+    <t>Nasi Kerabu</t>
+  </si>
+  <si>
+    <t>Asam Pedas</t>
+  </si>
+  <si>
+    <t>Kuih Lapis</t>
+  </si>
+  <si>
+    <t>Rendang Ayam</t>
+  </si>
+  <si>
+    <t>Nasi Goreng</t>
+  </si>
+  <si>
+    <t>Soto Ayam</t>
+  </si>
+  <si>
+    <t>Curry Puff</t>
   </si>
 </sst>
 </file>
@@ -1334,35 +1493,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1E0269-C437-A94E-8279-C3E013FE070B}">
   <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5:W18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.19921875" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" customWidth="1"/>
+    <col min="3" max="3" width="21.69921875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.296875" customWidth="1"/>
+    <col min="6" max="6" width="14.296875" customWidth="1"/>
+    <col min="7" max="7" width="12.796875" customWidth="1"/>
+    <col min="8" max="8" width="16.69921875" customWidth="1"/>
+    <col min="9" max="9" width="14.796875" customWidth="1"/>
+    <col min="10" max="10" width="14.19921875" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" customWidth="1"/>
-    <col min="24" max="24" width="13.83203125" customWidth="1"/>
-    <col min="25" max="25" width="15.33203125" customWidth="1"/>
-    <col min="28" max="28" width="19.83203125" customWidth="1"/>
+    <col min="13" max="13" width="20.296875" customWidth="1"/>
+    <col min="14" max="14" width="15.19921875" customWidth="1"/>
+    <col min="15" max="15" width="17.796875" customWidth="1"/>
+    <col min="16" max="16" width="20.09765625" customWidth="1"/>
+    <col min="17" max="17" width="16.796875" customWidth="1"/>
+    <col min="19" max="19" width="19.5" customWidth="1"/>
+    <col min="21" max="21" width="13.69921875" customWidth="1"/>
+    <col min="23" max="23" width="20.19921875" customWidth="1"/>
+    <col min="24" max="24" width="13.796875" customWidth="1"/>
+    <col min="25" max="25" width="15.296875" customWidth="1"/>
+    <col min="28" max="28" width="19.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1455,10 +1616,10 @@
       </c>
       <c r="AE1" s="3"/>
     </row>
-    <row r="2" spans="1:31" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:31" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1550,7 +1711,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1603,7 +1764,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1637,14 +1798,23 @@
       <c r="M5" t="s">
         <v>71</v>
       </c>
+      <c r="P5" t="s">
+        <v>289</v>
+      </c>
       <c r="Q5" s="7" t="s">
         <v>280</v>
       </c>
+      <c r="S5" t="s">
+        <v>309</v>
+      </c>
+      <c r="W5" t="s">
+        <v>328</v>
+      </c>
       <c r="AB5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1672,11 +1842,20 @@
       <c r="M6" t="s">
         <v>249</v>
       </c>
+      <c r="P6" t="s">
+        <v>290</v>
+      </c>
       <c r="Q6" s="7" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="S6" t="s">
+        <v>310</v>
+      </c>
+      <c r="W6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1704,11 +1883,20 @@
       <c r="M7" t="s">
         <v>250</v>
       </c>
+      <c r="P7" t="s">
+        <v>291</v>
+      </c>
       <c r="Q7" s="7" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="S7" t="s">
+        <v>311</v>
+      </c>
+      <c r="W7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1736,11 +1924,20 @@
       <c r="M8" t="s">
         <v>251</v>
       </c>
+      <c r="P8" t="s">
+        <v>292</v>
+      </c>
       <c r="Q8" s="7" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>312</v>
+      </c>
+      <c r="W8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1768,11 +1965,20 @@
       <c r="M9" t="s">
         <v>55</v>
       </c>
+      <c r="P9" t="s">
+        <v>293</v>
+      </c>
       <c r="Q9" s="7" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="S9" t="s">
+        <v>313</v>
+      </c>
+      <c r="W9" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1797,11 +2003,20 @@
       <c r="M10" t="s">
         <v>253</v>
       </c>
+      <c r="P10" t="s">
+        <v>294</v>
+      </c>
       <c r="Q10" s="7" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="S10" t="s">
+        <v>314</v>
+      </c>
+      <c r="W10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -1826,11 +2041,20 @@
       <c r="M11" t="s">
         <v>254</v>
       </c>
+      <c r="P11" t="s">
+        <v>295</v>
+      </c>
       <c r="Q11" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>315</v>
+      </c>
+      <c r="W11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1855,11 +2079,20 @@
       <c r="M12" t="s">
         <v>259</v>
       </c>
+      <c r="P12" t="s">
+        <v>296</v>
+      </c>
       <c r="Q12" s="7" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="S12" t="s">
+        <v>316</v>
+      </c>
+      <c r="W12" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -1884,8 +2117,17 @@
       <c r="M13" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="P13" t="s">
+        <v>297</v>
+      </c>
+      <c r="S13" t="s">
+        <v>317</v>
+      </c>
+      <c r="W13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -1910,8 +2152,17 @@
       <c r="M14" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="P14" t="s">
+        <v>298</v>
+      </c>
+      <c r="S14" t="s">
+        <v>318</v>
+      </c>
+      <c r="W14" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -1936,8 +2187,17 @@
       <c r="M15" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="P15" t="s">
+        <v>299</v>
+      </c>
+      <c r="S15" t="s">
+        <v>319</v>
+      </c>
+      <c r="W15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -1962,8 +2222,17 @@
       <c r="M16" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P16" t="s">
+        <v>300</v>
+      </c>
+      <c r="S16" t="s">
+        <v>320</v>
+      </c>
+      <c r="W16" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -1988,8 +2257,17 @@
       <c r="M17" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S17" t="s">
+        <v>321</v>
+      </c>
+      <c r="W17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -2011,8 +2289,17 @@
       <c r="L18" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P18" t="s">
+        <v>302</v>
+      </c>
+      <c r="S18" t="s">
+        <v>322</v>
+      </c>
+      <c r="W18" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -2034,8 +2321,14 @@
       <c r="L19" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P19" t="s">
+        <v>303</v>
+      </c>
+      <c r="S19" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -2054,8 +2347,14 @@
       <c r="J20" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P20" t="s">
+        <v>304</v>
+      </c>
+      <c r="S20" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>158</v>
       </c>
@@ -2074,8 +2373,14 @@
       <c r="L21" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P21" t="s">
+        <v>305</v>
+      </c>
+      <c r="S21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>159</v>
       </c>
@@ -2094,8 +2399,14 @@
       <c r="L22" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P22" t="s">
+        <v>306</v>
+      </c>
+      <c r="S22" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>160</v>
       </c>
@@ -2111,8 +2422,14 @@
       <c r="J23" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P23" t="s">
+        <v>307</v>
+      </c>
+      <c r="S23" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>161</v>
       </c>
@@ -2122,8 +2439,11 @@
       <c r="E24" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>162</v>
       </c>
@@ -2137,7 +2457,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>163</v>
       </c>
@@ -2151,7 +2471,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>164</v>
       </c>
@@ -2165,7 +2485,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>165</v>
       </c>
@@ -2179,7 +2499,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>288</v>
       </c>
@@ -2193,7 +2513,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>195</v>
       </c>
@@ -2204,7 +2524,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>196</v>
       </c>
@@ -2215,7 +2535,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>197</v>
       </c>
@@ -2226,7 +2546,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>198</v>
       </c>
@@ -2237,7 +2557,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>199</v>
       </c>
@@ -2245,7 +2565,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>200</v>
       </c>
@@ -2253,7 +2573,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:10" ht="20.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>201</v>
       </c>
@@ -2261,7 +2581,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
         <v>202</v>
       </c>
@@ -2269,62 +2589,62 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E41" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E42" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E43" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E44" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E45" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E46" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E47" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" t="s">
         <v>153</v>
       </c>

</xml_diff>